<commit_message>
cambio a mensaje a nonimo
</commit_message>
<xml_diff>
--- a/titulos_enviados_11-02-2025.xlsx
+++ b/titulos_enviados_11-02-2025.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A40"/>
+  <dimension ref="A1:A61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -713,6 +713,153 @@
         </is>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Alpura Selecta Leche Entera Deslactosada 100% de Vaca, Ultrapasteurizada en paquete de 12 Piezas de 1 Litro cada una, de fácil digestión, Fuente de proteína y Calcio, adicionada con vitaminas A y D. Cremosidad y Sabor superior</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Lámpara Escritorio LED,Lámpara de Oficina,Lámpara de Mesa con Atenuación de Protección para Los Ojos,Luz de Lectura con Usb Recargable,3 Colores con Clip,360 ° Flexión,para Trabajar, Estudiar, Leer</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Lámpara Escritorio LED,Lámpara de Oficina,Lámpara de Mesa con Atenuación de Protección para Los Ojos,Luz de Lectura con Usb Recargable,3 Colores con Clip,360 ° Flexión,para Trabajar, Estudiar, Leer</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Govee Tira LED 20 Metros, Cinta LED WiFi Compatible con Alexa, Sync de Música, Bricolaje de Múltiples Colores en Una Línea para Habitación, Decoracion de Año Nuevo</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>UGREEN 2M Cable USB C a USB A 2.0, 3A USB C Cable Tipo C Carga Rápida con Trenza de Nailon, Cable USB Tipo C Compatible con iPhone 16 15 Pro Max Plus, Galaxy S24 S23 S22 S21, Redmi, Pixel, Huawei</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>UGREEN 2M Cable USB C a USB A 2.0, 3A USB C Cable Tipo C Carga Rápida con Trenza de Nailon, Cable USB Tipo C Compatible con iPhone 16 15 Pro Max Plus, Galaxy S24 S23 S22 S21, Redmi, Pixel, Huawei</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>PUMA - Sudadera de forro polar con cuello redondo para mujer (negro, L), Negro -, Large</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Cómo mandar a la mierda de forma educada</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Zombieland: Double Tap - Roadtrip - PS4 - Estándar Edition</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Milky Way chocolate 14 barras de 48 g c/u, Total 672g</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Simple Wisdom Escritorio Minimalista,Escritorio con Repisa En Casa 1.2m,DiseñO Minimalista Moderno Escritorio Oficina,（120cm*50cm） (Blanco Puro)</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2pcs Lámpara de Techo 36W ，Wodoso Lampara de Techo LED Empotrable，3000K-6500K，30CM,Con Mando a Distancia, Compatible con app</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Porta de Pasaporte de Cuero PU, Funda para Pasaporte con Bloqueo RFID, Billetera de pasaporte, Titular de Pasaporte de Billetera de Viajes con Soporte para la Pluma para Mujeres/Hombres (Amarillo)</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Santa Clara - Leche Deslactosada Light, 12 Pack de 1 Lt cada uno</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>WERA - 05051493001-838 RA-R M Destornillador de bitholding con función de carraca, 1/4", 1/4" x 123,5 mm</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>SlowTon Quitapelos y Rodillos para Mascotas, Cepillo de Limpieza Removedor de Pelaje para Perros y Gatos, Reutilizable Rodillo Quita Pelos, Eliminador de Pelo para Animales Cepillos para Perros(Azure)</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Casio Serie A158WA | Reloj digital unisex | clásico | WR | Cronómetro 100 SEC | Alarma diaria | Mantenimiento de tiempo regular: hora, minuto, segundo, pm, fecha, día | Luz LED | Batería de 7 años</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>amiibo Toad Super Mario Series</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Perras de reserva</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>ACOVARK Funda para Samsung Galaxy S24 Ultra 5G,con 3piezas de película Protectora de Alta adherencia, magnético Anti-Amarillo Antigolpes Protectora Carcasa,Ultrafino y tecnológico,protección Ocular</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Fresh Step Multi-Cat con el Poder de Febreze, Arena para Gatos aglutinante de 14 LB/ 6.35 Kg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>